<commit_message>
Everything working until I tried to use paul_resources in the Paulthon/Option_Scraper file, and got the FileNotFoundError. From here, I rearrange my files, separating out the pkl and csv files from python files.
</commit_message>
<xml_diff>
--- a/CLVS_RiskScenarios2.xlsx
+++ b/CLVS_RiskScenarios2.xlsx
@@ -9,8 +9,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sub_States" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sub_States_Copy" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Summary" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Summary" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sub_States_Copy" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Core_Scenarios" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Multi" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Main" sheetId="6" state="visible" r:id="rId7"/>
@@ -326,8 +326,8 @@
   <numFmts count="8">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.00"/>
-    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.00"/>
     <numFmt numFmtId="168" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="169" formatCode="0.00%"/>
     <numFmt numFmtId="170" formatCode="#,##0.00000"/>
@@ -636,11 +636,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -656,11 +656,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -668,11 +668,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -688,11 +688,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -700,11 +700,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -744,23 +744,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -780,7 +780,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -788,15 +788,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="17" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="17" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -804,11 +804,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -816,7 +816,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -900,19 +900,19 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -945,17 +945,18 @@
         <v>Clean Approval</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>0.7</v>
+        <f aca="false">F2/SUM($F$2:$F$3)</f>
+        <v>0.998996990972919</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
       <c r="E2" s="1" t="n">
         <f aca="false">1+D2</f>
-        <v>1.1</v>
+        <v>1.03</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>0.55</v>
+        <v>0.996</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -966,18 +967,17 @@
       </c>
       <c r="C3" s="1" t="n">
         <f aca="false">F3/SUM($F$2:$F$3)</f>
-        <v>0.45</v>
+        <v>0.00100300902708124</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1" t="n">
         <f aca="false">1+D3</f>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F3" s="1" t="n">
-        <f aca="false">1-F2</f>
-        <v>0.45</v>
+        <v>0.001</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -990,20 +990,19 @@
         <f aca="false">Multi!A20</f>
         <v>CRL - Minor Delay</v>
       </c>
-      <c r="C4" s="1" t="e">
+      <c r="C4" s="1" t="n">
         <f aca="false">F4/SUM($F$4:$F$6)</f>
-        <v>#DIV/0!</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="D4" s="1" t="n">
-        <f aca="false">$D$3</f>
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1" t="n">
         <f aca="false">1+D4</f>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="G4" s="1"/>
     </row>
@@ -1013,19 +1012,18 @@
         <v>CRL - Major Delay</v>
       </c>
       <c r="C5" s="1" t="n">
-        <f aca="false">Multi!J21</f>
-        <v>0.25</v>
+        <f aca="false">F5/SUM($F$4:$F$6)</f>
+        <v>0.333333333333333</v>
       </c>
       <c r="D5" s="1" t="n">
-        <f aca="false">$D$3</f>
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1" t="n">
         <f aca="false">1+D5</f>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -1035,19 +1033,19 @@
         <v>CRL - No Hope</v>
       </c>
       <c r="C6" s="1" t="n">
-        <f aca="false">Multi!J22</f>
-        <v>0.15</v>
+        <f aca="false">F6/SUM($F$4:$F$6)</f>
+        <v>0.333333333333334</v>
       </c>
       <c r="D6" s="1" t="n">
-        <f aca="false">$D$3</f>
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1" t="n">
         <f aca="false">1+D6</f>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>0</v>
+        <f aca="false">1-F2-F3-F4-F5</f>
+        <v>0.001</v>
       </c>
       <c r="G6" s="1"/>
     </row>
@@ -1075,7 +1073,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1104,7 +1102,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
@@ -1112,148 +1110,106 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1734693877551"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <f aca="false">Sub_States!F2+Sub_States!F3</f>
+        <v>0.997</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <f aca="false">SUMPRODUCT(Sub_States!C2:C3,Sub_States!D2:D3)</f>
+        <v>0.0299699097291876</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <f aca="false">Sub_States!F4+Sub_States!F5+Sub_States!F6</f>
+        <v>0.003</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <f aca="false">SUMPRODUCT(Sub_States!C4:C6,Sub_States!D4:D6)</f>
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="n">
+        <f aca="false">SUM(B2:B3)</f>
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="str">
-        <f aca="false">Multi!A8</f>
-        <v>Positive</v>
-      </c>
-      <c r="B2" s="0" t="str">
-        <f aca="false">Multi!A15</f>
-        <v>Clean Approval</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <f aca="false">F2/SUM($F$2:$F$3)</f>
-        <v>0.767441860465116</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <f aca="false">1+D2</f>
-        <v>1.15</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <v>0.66</v>
-      </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="str">
-        <f aca="false">Multi!A16</f>
-        <v>Approved</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <f aca="false">F3/SUM($F$2:$F$3)</f>
-        <v>0.232558139534884</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <f aca="false">1+D3</f>
-        <v>1.05</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="str">
-        <f aca="false">Multi!A9</f>
-        <v>Negative</v>
-      </c>
-      <c r="B4" s="0" t="str">
-        <f aca="false">Multi!A20</f>
-        <v>CRL - Minor Delay</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <f aca="false">F4/SUM($F$4:$F$6)</f>
-        <v>0.620689655172414</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>-0.15</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <f aca="false">1+D4</f>
-        <v>0.85</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="G4" s="1"/>
+      <c r="C4" s="2" t="n">
+        <f aca="false">SUMPRODUCT(B2:B3,C2:C3)</f>
+        <v>0.02988</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="str">
-        <f aca="false">Multi!A21</f>
-        <v>CRL - Major Delay</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <f aca="false">Multi!J21</f>
-        <v>0.25</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>-0.25</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <f aca="false">1+D5</f>
-        <v>0.75</v>
-      </c>
-      <c r="F5" s="1" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="G5" s="1"/>
+      <c r="A5" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="str">
-        <f aca="false">Multi!A22</f>
-        <v>CRL - No Hope</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <f aca="false">Multi!J22</f>
-        <v>0.15</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>-0.4</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <f aca="false">1+D6</f>
-        <v>0.6</v>
-      </c>
-      <c r="F6" s="1" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="G6" s="1"/>
+      <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="e">
+        <f aca="false">-C2/C3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <f aca="false">B2</f>
+        <v>0.997</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <f aca="false">B3</f>
+        <v>0.003</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="0" t="e">
+        <f aca="false">(B6*B7-B8)/B6</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3" t="e">
+        <f aca="false">B9*(1/-C3)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1271,115 +1227,156 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B52" activeCellId="0" sqref="B52"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <f aca="false">Sub_States!F2+Sub_States!F3</f>
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <f aca="false">SUMPRODUCT(Sub_States!C2:C3,Sub_States!D2:D3)</f>
-        <v>0.025</v>
-      </c>
+      <c r="A2" s="0" t="str">
+        <f aca="false">Multi!A8</f>
+        <v>Positive</v>
+      </c>
+      <c r="B2" s="0" t="str">
+        <f aca="false">Multi!A15</f>
+        <v>Clean Approval</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <f aca="false">F2/SUM($F$2:$F$3)</f>
+        <v>0.767441860465116</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <f aca="false">1+D2</f>
+        <v>1.15</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <f aca="false">Sub_States!F4+Sub_States!F5+Sub_States!F6</f>
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="e">
-        <f aca="false">SUMPRODUCT(Sub_States!C4:C6,Sub_States!D4:D6)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="B3" s="0" t="str">
+        <f aca="false">Multi!A16</f>
+        <v>Approved</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <f aca="false">F3/SUM($F$2:$F$3)</f>
+        <v>0.232558139534884</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <f aca="false">1+D3</f>
+        <v>1.05</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="n">
-        <f aca="false">SUM(B2:B3)</f>
-        <v>1</v>
-      </c>
-      <c r="C4" s="0" t="e">
-        <f aca="false">SUMPRODUCT(B2:B3,C2:C3)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="A4" s="0" t="str">
+        <f aca="false">Multi!A9</f>
+        <v>Negative</v>
+      </c>
+      <c r="B4" s="0" t="str">
+        <f aca="false">Multi!A20</f>
+        <v>CRL - Minor Delay</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <f aca="false">F4/SUM($F$4:$F$6)</f>
+        <v>0.620689655172414</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>-0.15</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <f aca="false">1+D4</f>
+        <v>0.85</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>9</v>
-      </c>
+      <c r="B5" s="0" t="str">
+        <f aca="false">Multi!A21</f>
+        <v>CRL - Major Delay</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <f aca="false">Multi!J21</f>
+        <v>0.25</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>-0.25</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <f aca="false">1+D5</f>
+        <v>0.75</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="0" t="e">
-        <f aca="false">-C2/C3</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <f aca="false">B2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <f aca="false">B3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="0" t="e">
-        <f aca="false">(B6*B7-B8)/B6</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="2" t="e">
-        <f aca="false">B9*(1/-C3)</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="B6" s="0" t="str">
+        <f aca="false">Multi!A22</f>
+        <v>CRL - No Hope</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <f aca="false">Multi!J22</f>
+        <v>0.15</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>-0.4</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <f aca="false">1+D6</f>
+        <v>0.6</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="G6" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1405,8 +1402,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1425,11 +1422,11 @@
         <f aca="false">Multi!A8</f>
         <v>Positive</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="2" t="n">
         <f aca="false">Multi!B8</f>
         <v>0.777777777777778</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="2" t="n">
         <f aca="false">Multi!C8</f>
         <v>0.0562499999999999</v>
       </c>
@@ -1439,11 +1436,11 @@
         <f aca="false">Multi!A9</f>
         <v>Negative</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="2" t="n">
         <f aca="false">Multi!B9</f>
         <v>0.222222222222222</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="2" t="n">
         <f aca="false">Multi!C9</f>
         <v>-0.196875</v>
       </c>
@@ -1472,15 +1469,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1574,11 +1571,11 @@
       <c r="A8" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="2" t="n">
         <f aca="false">(B3-D9)/(D8-D9)</f>
         <v>0.777777777777778</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="2" t="n">
         <f aca="false">D8/$B$3-1</f>
         <v>0.0562499999999999</v>
       </c>
@@ -1593,7 +1590,7 @@
       <c r="I8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="3" t="n">
+      <c r="J8" s="2" t="n">
         <v>0.7</v>
       </c>
       <c r="K8" s="5" t="n">
@@ -1613,11 +1610,11 @@
       <c r="A9" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="3" t="n">
+      <c r="B9" s="2" t="n">
         <f aca="false">1-B8</f>
         <v>0.222222222222222</v>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" s="2" t="n">
         <f aca="false">D9/$B$3-1</f>
         <v>-0.196875</v>
       </c>
@@ -1632,7 +1629,7 @@
       <c r="I9" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="3" t="n">
+      <c r="J9" s="2" t="n">
         <f aca="false">1-J8</f>
         <v>0.3</v>
       </c>
@@ -1690,26 +1687,26 @@
       <c r="A15" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="3" t="n">
+      <c r="B15" s="2" t="n">
         <f aca="false">$B$8*J15</f>
         <v>0.622222222222222</v>
       </c>
-      <c r="C15" s="3" t="n">
+      <c r="C15" s="2" t="n">
         <f aca="false">K15/$B$3-1</f>
         <v>0.0625</v>
       </c>
-      <c r="D15" s="3" t="n">
+      <c r="D15" s="2" t="n">
         <f aca="false">L15/$B$3-1</f>
         <v>0.03125</v>
       </c>
-      <c r="E15" s="3" t="n">
+      <c r="E15" s="2" t="n">
         <f aca="false">M15/$B$3-1</f>
         <v>0.25</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>0.025</v>
       </c>
-      <c r="J15" s="3" t="n">
+      <c r="J15" s="2" t="n">
         <v>0.8</v>
       </c>
       <c r="K15" s="4" t="n">
@@ -1730,19 +1727,19 @@
       <c r="A16" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="3" t="n">
+      <c r="B16" s="2" t="n">
         <f aca="false">$B$8*J16</f>
         <v>0.155555555555556</v>
       </c>
-      <c r="C16" s="3" t="n">
+      <c r="C16" s="2" t="n">
         <f aca="false">K16/$B$3-1</f>
         <v>0.03125</v>
       </c>
-      <c r="D16" s="3" t="n">
+      <c r="D16" s="2" t="n">
         <f aca="false">L16/$B$3-1</f>
         <v>0.0125</v>
       </c>
-      <c r="E16" s="3" t="n">
+      <c r="E16" s="2" t="n">
         <f aca="false">M16/$B$3-1</f>
         <v>0.09375</v>
       </c>
@@ -1750,7 +1747,7 @@
         <f aca="false">$F$15</f>
         <v>0.025</v>
       </c>
-      <c r="J16" s="3" t="n">
+      <c r="J16" s="2" t="n">
         <f aca="false">1-J15</f>
         <v>0.2</v>
       </c>
@@ -1803,19 +1800,19 @@
       <c r="A20" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="3" t="n">
+      <c r="B20" s="2" t="n">
         <f aca="false">J20*$B$9</f>
         <v>0.133333333333333</v>
       </c>
-      <c r="C20" s="3" t="n">
+      <c r="C20" s="2" t="n">
         <f aca="false">K20/$B$3-1</f>
         <v>-0.125</v>
       </c>
-      <c r="D20" s="3" t="n">
+      <c r="D20" s="2" t="n">
         <f aca="false">L20/$B$3-1</f>
         <v>-0.1875</v>
       </c>
-      <c r="E20" s="3" t="n">
+      <c r="E20" s="2" t="n">
         <f aca="false">M20/$B$3-1</f>
         <v>-0.0625</v>
       </c>
@@ -1823,7 +1820,7 @@
         <f aca="false">$F$15</f>
         <v>0.025</v>
       </c>
-      <c r="J20" s="3" t="n">
+      <c r="J20" s="2" t="n">
         <v>0.6</v>
       </c>
       <c r="K20" s="4" t="n">
@@ -1844,19 +1841,19 @@
       <c r="A21" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="3" t="n">
+      <c r="B21" s="2" t="n">
         <f aca="false">J21*$B$9</f>
         <v>0.0555555555555556</v>
       </c>
-      <c r="C21" s="3" t="n">
+      <c r="C21" s="2" t="n">
         <f aca="false">K21/$B$3-1</f>
         <v>-0.1875</v>
       </c>
-      <c r="D21" s="3" t="n">
+      <c r="D21" s="2" t="n">
         <f aca="false">L21/$B$3-1</f>
         <v>-0.25</v>
       </c>
-      <c r="E21" s="3" t="n">
+      <c r="E21" s="2" t="n">
         <f aca="false">M21/$B$3-1</f>
         <v>-0.125</v>
       </c>
@@ -1864,7 +1861,7 @@
         <f aca="false">$F$15</f>
         <v>0.025</v>
       </c>
-      <c r="J21" s="3" t="n">
+      <c r="J21" s="2" t="n">
         <v>0.25</v>
       </c>
       <c r="K21" s="4" t="n">
@@ -1885,19 +1882,19 @@
       <c r="A22" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="3" t="n">
+      <c r="B22" s="2" t="n">
         <f aca="false">J22*$B$9</f>
         <v>0.0333333333333333</v>
       </c>
-      <c r="C22" s="3" t="n">
+      <c r="C22" s="2" t="n">
         <f aca="false">K22/$B$3-1</f>
         <v>-0.5</v>
       </c>
-      <c r="D22" s="3" t="n">
+      <c r="D22" s="2" t="n">
         <f aca="false">L22/$B$3-1</f>
         <v>-0.5625</v>
       </c>
-      <c r="E22" s="3" t="n">
+      <c r="E22" s="2" t="n">
         <f aca="false">M22/$B$3-1</f>
         <v>-0.375</v>
       </c>
@@ -1905,7 +1902,7 @@
         <f aca="false">$F$15</f>
         <v>0.025</v>
       </c>
-      <c r="J22" s="3" t="n">
+      <c r="J22" s="2" t="n">
         <f aca="false">1-J20-J21</f>
         <v>0.15</v>
       </c>
@@ -1929,11 +1926,11 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D24" s="3" t="n">
+      <c r="D24" s="2" t="n">
         <f aca="false">SQRT(SUMPRODUCT(D26:D50*E26:E50^2))</f>
         <v>0.125353385024708</v>
       </c>
-      <c r="O24" s="3" t="n">
+      <c r="O24" s="2" t="n">
         <f aca="false">SQRT(SUMPRODUCT(N26:N50*O26:O50^2))</f>
         <v>0.13917821730384</v>
       </c>
@@ -2021,7 +2018,7 @@
       <c r="J26" s="13" t="n">
         <v>0.1</v>
       </c>
-      <c r="K26" s="3" t="n">
+      <c r="K26" s="2" t="n">
         <f aca="false">$J$15</f>
         <v>0.8</v>
       </c>
@@ -2029,7 +2026,7 @@
         <f aca="false">C26+($M$8-$E$8)</f>
         <v>90.825</v>
       </c>
-      <c r="N26" s="3" t="n">
+      <c r="N26" s="2" t="n">
         <f aca="false">K26*$J$8*J26</f>
         <v>0.056</v>
       </c>
@@ -2069,14 +2066,14 @@
         <f aca="false">$F$15</f>
         <v>0.025</v>
       </c>
-      <c r="I27" s="3" t="n">
+      <c r="I27" s="2" t="n">
         <f aca="false">$B$15</f>
         <v>0.622222222222222</v>
       </c>
       <c r="J27" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="K27" s="3" t="n">
+      <c r="K27" s="2" t="n">
         <f aca="false">$J$15</f>
         <v>0.8</v>
       </c>
@@ -2084,7 +2081,7 @@
         <f aca="false">C27+($M$8-$E$8)</f>
         <v>88.7</v>
       </c>
-      <c r="N27" s="3" t="n">
+      <c r="N27" s="2" t="n">
         <f aca="false">K27*$J$8*J27</f>
         <v>0.112</v>
       </c>
@@ -2118,14 +2115,14 @@
         <f aca="false">$F$15</f>
         <v>0.025</v>
       </c>
-      <c r="I28" s="3" t="n">
+      <c r="I28" s="2" t="n">
         <f aca="false">$B$15</f>
         <v>0.622222222222222</v>
       </c>
       <c r="J28" s="0" t="n">
         <v>0.4</v>
       </c>
-      <c r="K28" s="3" t="n">
+      <c r="K28" s="2" t="n">
         <f aca="false">$J$15</f>
         <v>0.8</v>
       </c>
@@ -2133,7 +2130,7 @@
         <f aca="false">C28+($M$8-$E$8)</f>
         <v>86.575</v>
       </c>
-      <c r="N28" s="3" t="n">
+      <c r="N28" s="2" t="n">
         <f aca="false">K28*$J$8*J28</f>
         <v>0.224</v>
       </c>
@@ -2167,14 +2164,14 @@
         <f aca="false">$F$15</f>
         <v>0.025</v>
       </c>
-      <c r="I29" s="3" t="n">
+      <c r="I29" s="2" t="n">
         <f aca="false">$B$15</f>
         <v>0.622222222222222</v>
       </c>
       <c r="J29" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="K29" s="3" t="n">
+      <c r="K29" s="2" t="n">
         <f aca="false">$J$15</f>
         <v>0.8</v>
       </c>
@@ -2182,7 +2179,7 @@
         <f aca="false">C29+($M$8-$E$8)</f>
         <v>84.45</v>
       </c>
-      <c r="N29" s="3" t="n">
+      <c r="N29" s="2" t="n">
         <f aca="false">K29*$J$8*J29</f>
         <v>0.112</v>
       </c>
@@ -2216,14 +2213,14 @@
         <f aca="false">$F$15</f>
         <v>0.025</v>
       </c>
-      <c r="I30" s="3" t="n">
+      <c r="I30" s="2" t="n">
         <f aca="false">$B$15</f>
         <v>0.622222222222222</v>
       </c>
       <c r="J30" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="K30" s="3" t="n">
+      <c r="K30" s="2" t="n">
         <f aca="false">$J$15</f>
         <v>0.8</v>
       </c>
@@ -2231,7 +2228,7 @@
         <f aca="false">C30+($M$8-$E$8)</f>
         <v>82.325</v>
       </c>
-      <c r="N30" s="3" t="n">
+      <c r="N30" s="2" t="n">
         <f aca="false">K30*$J$8*J30</f>
         <v>0.056</v>
       </c>
@@ -2279,7 +2276,7 @@
       <c r="J31" s="13" t="n">
         <v>0.1</v>
       </c>
-      <c r="K31" s="3" t="n">
+      <c r="K31" s="2" t="n">
         <f aca="false">$J$16</f>
         <v>0.2</v>
       </c>
@@ -2287,7 +2284,7 @@
         <f aca="false">C31+($M$8-$E$8)</f>
         <v>88.2</v>
       </c>
-      <c r="N31" s="3" t="n">
+      <c r="N31" s="2" t="n">
         <f aca="false">K31*$J$8*J31</f>
         <v>0.014</v>
       </c>
@@ -2327,14 +2324,14 @@
         <f aca="false">$F$16</f>
         <v>0.025</v>
       </c>
-      <c r="I32" s="3" t="n">
+      <c r="I32" s="2" t="n">
         <f aca="false">$B$16</f>
         <v>0.155555555555556</v>
       </c>
       <c r="J32" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="K32" s="3" t="n">
+      <c r="K32" s="2" t="n">
         <f aca="false">$J$16</f>
         <v>0.2</v>
       </c>
@@ -2342,7 +2339,7 @@
         <f aca="false">C32+($M$8-$E$8)</f>
         <v>86.1375</v>
       </c>
-      <c r="N32" s="3" t="n">
+      <c r="N32" s="2" t="n">
         <f aca="false">K32*$J$8*J32</f>
         <v>0.028</v>
       </c>
@@ -2376,14 +2373,14 @@
         <f aca="false">$F$16</f>
         <v>0.025</v>
       </c>
-      <c r="I33" s="3" t="n">
+      <c r="I33" s="2" t="n">
         <f aca="false">$B$16</f>
         <v>0.155555555555556</v>
       </c>
       <c r="J33" s="0" t="n">
         <v>0.4</v>
       </c>
-      <c r="K33" s="3" t="n">
+      <c r="K33" s="2" t="n">
         <f aca="false">$J$16</f>
         <v>0.2</v>
       </c>
@@ -2391,7 +2388,7 @@
         <f aca="false">C33+($M$8-$E$8)</f>
         <v>84.075</v>
       </c>
-      <c r="N33" s="3" t="n">
+      <c r="N33" s="2" t="n">
         <f aca="false">K33*$J$8*J33</f>
         <v>0.056</v>
       </c>
@@ -2425,14 +2422,14 @@
         <f aca="false">$F$16</f>
         <v>0.025</v>
       </c>
-      <c r="I34" s="3" t="n">
+      <c r="I34" s="2" t="n">
         <f aca="false">$B$16</f>
         <v>0.155555555555556</v>
       </c>
       <c r="J34" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="K34" s="3" t="n">
+      <c r="K34" s="2" t="n">
         <f aca="false">$J$16</f>
         <v>0.2</v>
       </c>
@@ -2440,7 +2437,7 @@
         <f aca="false">C34+($M$8-$E$8)</f>
         <v>82.0125</v>
       </c>
-      <c r="N34" s="3" t="n">
+      <c r="N34" s="2" t="n">
         <f aca="false">K34*$J$8*J34</f>
         <v>0.028</v>
       </c>
@@ -2474,14 +2471,14 @@
         <f aca="false">$F$16</f>
         <v>0.025</v>
       </c>
-      <c r="I35" s="3" t="n">
+      <c r="I35" s="2" t="n">
         <f aca="false">$B$16</f>
         <v>0.155555555555556</v>
       </c>
       <c r="J35" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="K35" s="3" t="n">
+      <c r="K35" s="2" t="n">
         <f aca="false">$J$16</f>
         <v>0.2</v>
       </c>
@@ -2489,7 +2486,7 @@
         <f aca="false">C35+($M$8-$E$8)</f>
         <v>79.95</v>
       </c>
-      <c r="N35" s="3" t="n">
+      <c r="N35" s="2" t="n">
         <f aca="false">K35*$J$8*J35</f>
         <v>0.014</v>
       </c>
@@ -2537,7 +2534,7 @@
       <c r="J36" s="13" t="n">
         <v>0.1</v>
       </c>
-      <c r="K36" s="3" t="n">
+      <c r="K36" s="2" t="n">
         <f aca="false">$J$20</f>
         <v>0.6</v>
       </c>
@@ -2545,7 +2542,7 @@
         <f aca="false">C36+($M$9-$E$9)</f>
         <v>75.075</v>
       </c>
-      <c r="N36" s="3" t="n">
+      <c r="N36" s="2" t="n">
         <f aca="false">K36*$J$9*J36</f>
         <v>0.018</v>
       </c>
@@ -2585,14 +2582,14 @@
         <f aca="false">$F$20</f>
         <v>0.025</v>
       </c>
-      <c r="I37" s="3" t="n">
+      <c r="I37" s="2" t="n">
         <f aca="false">$B$20</f>
         <v>0.133333333333333</v>
       </c>
       <c r="J37" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="K37" s="3" t="n">
+      <c r="K37" s="2" t="n">
         <f aca="false">$J$20</f>
         <v>0.6</v>
       </c>
@@ -2600,7 +2597,7 @@
         <f aca="false">C37+($M$9-$E$9)</f>
         <v>73.325</v>
       </c>
-      <c r="N37" s="3" t="n">
+      <c r="N37" s="2" t="n">
         <f aca="false">K37*$J$9*J37</f>
         <v>0.036</v>
       </c>
@@ -2634,14 +2631,14 @@
         <f aca="false">$F$20</f>
         <v>0.025</v>
       </c>
-      <c r="I38" s="3" t="n">
+      <c r="I38" s="2" t="n">
         <f aca="false">$B$20</f>
         <v>0.133333333333333</v>
       </c>
       <c r="J38" s="0" t="n">
         <v>0.4</v>
       </c>
-      <c r="K38" s="3" t="n">
+      <c r="K38" s="2" t="n">
         <f aca="false">$J$20</f>
         <v>0.6</v>
       </c>
@@ -2649,7 +2646,7 @@
         <f aca="false">C38+($M$9-$E$9)</f>
         <v>71.575</v>
       </c>
-      <c r="N38" s="3" t="n">
+      <c r="N38" s="2" t="n">
         <f aca="false">K38*$J$9*J38</f>
         <v>0.072</v>
       </c>
@@ -2683,14 +2680,14 @@
         <f aca="false">$F$20</f>
         <v>0.025</v>
       </c>
-      <c r="I39" s="3" t="n">
+      <c r="I39" s="2" t="n">
         <f aca="false">$B$20</f>
         <v>0.133333333333333</v>
       </c>
       <c r="J39" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="K39" s="3" t="n">
+      <c r="K39" s="2" t="n">
         <f aca="false">$J$20</f>
         <v>0.6</v>
       </c>
@@ -2698,7 +2695,7 @@
         <f aca="false">C39+($M$9-$E$9)</f>
         <v>69.825</v>
       </c>
-      <c r="N39" s="3" t="n">
+      <c r="N39" s="2" t="n">
         <f aca="false">K39*$J$9*J39</f>
         <v>0.036</v>
       </c>
@@ -2732,14 +2729,14 @@
         <f aca="false">$F$20</f>
         <v>0.025</v>
       </c>
-      <c r="I40" s="3" t="n">
+      <c r="I40" s="2" t="n">
         <f aca="false">$B$20</f>
         <v>0.133333333333333</v>
       </c>
       <c r="J40" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="K40" s="3" t="n">
+      <c r="K40" s="2" t="n">
         <f aca="false">$J$20</f>
         <v>0.6</v>
       </c>
@@ -2747,7 +2744,7 @@
         <f aca="false">C40+($M$9-$E$9)</f>
         <v>68.075</v>
       </c>
-      <c r="N40" s="3" t="n">
+      <c r="N40" s="2" t="n">
         <f aca="false">K40*$J$9*J40</f>
         <v>0.018</v>
       </c>
@@ -2795,7 +2792,7 @@
       <c r="J41" s="13" t="n">
         <v>0.1</v>
       </c>
-      <c r="K41" s="3" t="n">
+      <c r="K41" s="2" t="n">
         <f aca="false">$J$21</f>
         <v>0.25</v>
       </c>
@@ -2803,7 +2800,7 @@
         <f aca="false">C41+($M$9-$E$9)</f>
         <v>69.825</v>
       </c>
-      <c r="N41" s="3" t="n">
+      <c r="N41" s="2" t="n">
         <f aca="false">K41*$J$9*J41</f>
         <v>0.0075</v>
       </c>
@@ -2843,14 +2840,14 @@
         <f aca="false">$F$21</f>
         <v>0.025</v>
       </c>
-      <c r="I42" s="3" t="n">
+      <c r="I42" s="2" t="n">
         <f aca="false">$B$21</f>
         <v>0.0555555555555556</v>
       </c>
       <c r="J42" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="K42" s="3" t="n">
+      <c r="K42" s="2" t="n">
         <f aca="false">$J$21</f>
         <v>0.25</v>
       </c>
@@ -2858,7 +2855,7 @@
         <f aca="false">C42+($M$9-$E$9)</f>
         <v>68.2</v>
       </c>
-      <c r="N42" s="3" t="n">
+      <c r="N42" s="2" t="n">
         <f aca="false">K42*$J$9*J42</f>
         <v>0.015</v>
       </c>
@@ -2892,14 +2889,14 @@
         <f aca="false">$F$21</f>
         <v>0.025</v>
       </c>
-      <c r="I43" s="3" t="n">
+      <c r="I43" s="2" t="n">
         <f aca="false">$B$21</f>
         <v>0.0555555555555556</v>
       </c>
       <c r="J43" s="0" t="n">
         <v>0.4</v>
       </c>
-      <c r="K43" s="3" t="n">
+      <c r="K43" s="2" t="n">
         <f aca="false">$J$21</f>
         <v>0.25</v>
       </c>
@@ -2907,7 +2904,7 @@
         <f aca="false">C43+($M$9-$E$9)</f>
         <v>66.575</v>
       </c>
-      <c r="N43" s="3" t="n">
+      <c r="N43" s="2" t="n">
         <f aca="false">K43*$J$9*J43</f>
         <v>0.03</v>
       </c>
@@ -2941,14 +2938,14 @@
         <f aca="false">$F$21</f>
         <v>0.025</v>
       </c>
-      <c r="I44" s="3" t="n">
+      <c r="I44" s="2" t="n">
         <f aca="false">$B$21</f>
         <v>0.0555555555555556</v>
       </c>
       <c r="J44" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="K44" s="3" t="n">
+      <c r="K44" s="2" t="n">
         <f aca="false">$J$21</f>
         <v>0.25</v>
       </c>
@@ -2956,7 +2953,7 @@
         <f aca="false">C44+($M$9-$E$9)</f>
         <v>64.95</v>
       </c>
-      <c r="N44" s="3" t="n">
+      <c r="N44" s="2" t="n">
         <f aca="false">K44*$J$9*J44</f>
         <v>0.015</v>
       </c>
@@ -2990,14 +2987,14 @@
         <f aca="false">$F$21</f>
         <v>0.025</v>
       </c>
-      <c r="I45" s="3" t="n">
+      <c r="I45" s="2" t="n">
         <f aca="false">$B$21</f>
         <v>0.0555555555555556</v>
       </c>
       <c r="J45" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="K45" s="3" t="n">
+      <c r="K45" s="2" t="n">
         <f aca="false">$J$21</f>
         <v>0.25</v>
       </c>
@@ -3005,7 +3002,7 @@
         <f aca="false">C45+($M$9-$E$9)</f>
         <v>63.325</v>
       </c>
-      <c r="N45" s="3" t="n">
+      <c r="N45" s="2" t="n">
         <f aca="false">K45*$J$9*J45</f>
         <v>0.0075</v>
       </c>
@@ -3053,7 +3050,7 @@
       <c r="J46" s="13" t="n">
         <v>0.1</v>
       </c>
-      <c r="K46" s="3" t="n">
+      <c r="K46" s="2" t="n">
         <f aca="false">$J$22</f>
         <v>0.15</v>
       </c>
@@ -3061,7 +3058,7 @@
         <f aca="false">C46+($M$9-$E$9)</f>
         <v>43.575</v>
       </c>
-      <c r="N46" s="3" t="n">
+      <c r="N46" s="2" t="n">
         <f aca="false">K46*$J$9*J46</f>
         <v>0.0045</v>
       </c>
@@ -3101,14 +3098,14 @@
         <f aca="false">$F$22</f>
         <v>0.025</v>
       </c>
-      <c r="I47" s="3" t="n">
+      <c r="I47" s="2" t="n">
         <f aca="false">$B$22</f>
         <v>0.0333333333333333</v>
       </c>
       <c r="J47" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="K47" s="3" t="n">
+      <c r="K47" s="2" t="n">
         <f aca="false">$J$22</f>
         <v>0.15</v>
       </c>
@@ -3116,7 +3113,7 @@
         <f aca="false">C47+($M$9-$E$9)</f>
         <v>42.575</v>
       </c>
-      <c r="N47" s="3" t="n">
+      <c r="N47" s="2" t="n">
         <f aca="false">K47*$J$9*J47</f>
         <v>0.009</v>
       </c>
@@ -3150,14 +3147,14 @@
         <f aca="false">$F$22</f>
         <v>0.025</v>
       </c>
-      <c r="I48" s="3" t="n">
+      <c r="I48" s="2" t="n">
         <f aca="false">$B$22</f>
         <v>0.0333333333333333</v>
       </c>
       <c r="J48" s="0" t="n">
         <v>0.4</v>
       </c>
-      <c r="K48" s="3" t="n">
+      <c r="K48" s="2" t="n">
         <f aca="false">$J$22</f>
         <v>0.15</v>
       </c>
@@ -3165,7 +3162,7 @@
         <f aca="false">C48+($M$9-$E$9)</f>
         <v>41.575</v>
       </c>
-      <c r="N48" s="3" t="n">
+      <c r="N48" s="2" t="n">
         <f aca="false">K48*$J$9*J48</f>
         <v>0.018</v>
       </c>
@@ -3199,14 +3196,14 @@
         <f aca="false">$F$22</f>
         <v>0.025</v>
       </c>
-      <c r="I49" s="3" t="n">
+      <c r="I49" s="2" t="n">
         <f aca="false">$B$22</f>
         <v>0.0333333333333333</v>
       </c>
       <c r="J49" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="K49" s="3" t="n">
+      <c r="K49" s="2" t="n">
         <f aca="false">$J$22</f>
         <v>0.15</v>
       </c>
@@ -3214,7 +3211,7 @@
         <f aca="false">C49+($M$9-$E$9)</f>
         <v>40.575</v>
       </c>
-      <c r="N49" s="3" t="n">
+      <c r="N49" s="2" t="n">
         <f aca="false">K49*$J$9*J49</f>
         <v>0.009</v>
       </c>
@@ -3248,14 +3245,14 @@
         <f aca="false">$F$22</f>
         <v>0.025</v>
       </c>
-      <c r="I50" s="3" t="n">
+      <c r="I50" s="2" t="n">
         <f aca="false">$B$22</f>
         <v>0.0333333333333333</v>
       </c>
       <c r="J50" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="K50" s="3" t="n">
+      <c r="K50" s="2" t="n">
         <f aca="false">$J$22</f>
         <v>0.15</v>
       </c>
@@ -3263,7 +3260,7 @@
         <f aca="false">C50+($M$9-$E$9)</f>
         <v>39.575</v>
       </c>
-      <c r="N50" s="3" t="n">
+      <c r="N50" s="2" t="n">
         <f aca="false">K50*$J$9*J50</f>
         <v>0.0045</v>
       </c>
@@ -3296,11 +3293,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.26530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.12755102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3790,20 +3787,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4144,38 +4141,38 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="2"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="42" t="n">
         <f aca="false">SQRT(B9*C9^2 + B10*C10^2)</f>
         <v>0.158113883008419</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="3"/>
       <c r="G11" s="42" t="n">
         <f aca="false">SQRT(F9*G9^2 + F10*G10^2)</f>
         <v>0.316227766016838</v>
       </c>
-      <c r="J11" s="2"/>
+      <c r="J11" s="3"/>
       <c r="K11" s="42" t="n">
         <f aca="false">SQRT(J9*K9^2 + J10*K10^2)</f>
         <v>0.0612372435695794</v>
       </c>
-      <c r="N11" s="2"/>
+      <c r="N11" s="3"/>
       <c r="O11" s="42" t="n">
         <f aca="false">SQRT(N9*O9^2 + N10*O10^2)</f>
         <v>0.105</v>
       </c>
-      <c r="R11" s="2"/>
+      <c r="R11" s="3"/>
       <c r="S11" s="42" t="n">
         <f aca="false">SQRT(R9*S9^2 + R10*S10^2)</f>
         <v>0.175</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E12" s="2"/>
+      <c r="E12" s="3"/>
       <c r="F12" s="43"/>
-      <c r="H12" s="2"/>
+      <c r="H12" s="3"/>
       <c r="I12" s="43"/>
-      <c r="K12" s="2"/>
+      <c r="K12" s="3"/>
       <c r="L12" s="43"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4185,11 +4182,11 @@
       <c r="B13" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="3"/>
       <c r="F13" s="43"/>
-      <c r="H13" s="2"/>
+      <c r="H13" s="3"/>
       <c r="I13" s="43"/>
-      <c r="K13" s="2"/>
+      <c r="K13" s="3"/>
       <c r="L13" s="43"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4205,17 +4202,17 @@
       <c r="D14" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="2"/>
+      <c r="M14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="47" t="s">
@@ -4482,7 +4479,7 @@
       <c r="B47" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="C47" s="3" t="n">
+      <c r="C47" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D47" s="4" t="n">
@@ -4497,7 +4494,7 @@
       <c r="B48" s="4" t="n">
         <v>50</v>
       </c>
-      <c r="C48" s="3" t="n">
+      <c r="C48" s="2" t="n">
         <v>0.8</v>
       </c>
       <c r="D48" s="4" t="n">
@@ -4610,15 +4607,15 @@
       <c r="P52" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="Q52" s="3" t="n">
+      <c r="Q52" s="2" t="n">
         <f aca="false">(G52-$B$13)/$B$13</f>
         <v>0.125</v>
       </c>
-      <c r="R52" s="3" t="n">
+      <c r="R52" s="2" t="n">
         <f aca="false">(H52-$B$13)/$B$13</f>
         <v>0</v>
       </c>
-      <c r="S52" s="3" t="n">
+      <c r="S52" s="2" t="n">
         <f aca="false">(I52-$B$13)/$B$13</f>
         <v>0.375</v>
       </c>
@@ -4669,15 +4666,15 @@
       <c r="P53" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="Q53" s="3" t="n">
+      <c r="Q53" s="2" t="n">
         <f aca="false">(G53-$B$13)/$B$13</f>
         <v>-0.25</v>
       </c>
-      <c r="R53" s="3" t="n">
+      <c r="R53" s="2" t="n">
         <f aca="false">(H53-$B$13)/$B$13</f>
         <v>-0.375</v>
       </c>
-      <c r="S53" s="3" t="n">
+      <c r="S53" s="2" t="n">
         <f aca="false">(I53-$B$13)/$B$13</f>
         <v>-0.125</v>
       </c>
@@ -4719,10 +4716,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="4.72448979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4791,8 +4789,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4818,15 +4816,15 @@
         <f aca="false">Params!A16</f>
         <v>Up</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="2" t="n">
         <f aca="false">Params!B16</f>
         <v>0.1</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="2" t="n">
         <f aca="false">Params!C16</f>
         <v>0.025</v>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="2" t="n">
         <f aca="false">Params!D16</f>
         <v>0.25</v>
       </c>
@@ -4836,15 +4834,15 @@
         <f aca="false">Params!A17</f>
         <v>Down</v>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="2" t="n">
         <f aca="false">Params!B17</f>
         <v>-0.25</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="2" t="n">
         <f aca="false">Params!C17</f>
         <v>-0.4</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="2" t="n">
         <f aca="false">Params!D17</f>
         <v>-0.15</v>
       </c>

</xml_diff>